<commit_message>
add and modify files
</commit_message>
<xml_diff>
--- a/Parametercombinations.xlsx
+++ b/Parametercombinations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkoenig\sciebo2\Forschung\Promotion\Paper_1\MCD-variogram-estimation-paper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkoenig\sciebo2\Forschung\Promotion\Paper_1\R-Code\MCD-variogram-estimation-paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$E$1:$E$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$E$1:$E$53</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -371,10 +371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -771,10 +771,10 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -794,16 +794,16 @@
         <v>1</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -823,16 +823,16 @@
         <v>1</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -858,7 +858,7 @@
         <v>1</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E17">
         <v>2</v>
@@ -887,16 +887,16 @@
         <v>1</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -916,16 +916,16 @@
         <v>1</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -945,16 +945,16 @@
         <v>1</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -974,16 +974,16 @@
         <v>1</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -1003,7 +1003,7 @@
         <v>1</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E22">
         <v>3</v>
@@ -1012,7 +1012,7 @@
         <v>2</v>
       </c>
       <c r="G22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -1032,7 +1032,7 @@
         <v>1</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E23">
         <v>3</v>
@@ -1041,7 +1041,7 @@
         <v>3</v>
       </c>
       <c r="G23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -1061,7 +1061,7 @@
         <v>1</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E24">
         <v>3</v>
@@ -1070,7 +1070,7 @@
         <v>4</v>
       </c>
       <c r="G24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -1090,7 +1090,7 @@
         <v>1</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E25">
         <v>3</v>
@@ -1099,7 +1099,7 @@
         <v>5</v>
       </c>
       <c r="G25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -1119,7 +1119,7 @@
         <v>1</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E26">
         <v>3</v>
@@ -1128,7 +1128,7 @@
         <v>2</v>
       </c>
       <c r="G26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -1148,7 +1148,7 @@
         <v>1</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E27">
         <v>3</v>
@@ -1157,7 +1157,7 @@
         <v>3</v>
       </c>
       <c r="G27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -1177,7 +1177,7 @@
         <v>1</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E28">
         <v>3</v>
@@ -1186,7 +1186,7 @@
         <v>4</v>
       </c>
       <c r="G28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -1206,7 +1206,7 @@
         <v>1</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E29">
         <v>3</v>
@@ -1215,7 +1215,7 @@
         <v>5</v>
       </c>
       <c r="G29">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -1235,7 +1235,7 @@
         <v>1</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E30">
         <v>3</v>
@@ -1244,7 +1244,7 @@
         <v>2</v>
       </c>
       <c r="G30">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -1264,7 +1264,7 @@
         <v>1</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E31">
         <v>3</v>
@@ -1273,7 +1273,7 @@
         <v>3</v>
       </c>
       <c r="G31">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -1293,7 +1293,7 @@
         <v>1</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E32">
         <v>3</v>
@@ -1302,7 +1302,7 @@
         <v>4</v>
       </c>
       <c r="G32">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -1322,7 +1322,7 @@
         <v>1</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E33">
         <v>3</v>
@@ -1331,7 +1331,7 @@
         <v>5</v>
       </c>
       <c r="G33">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H33">
         <v>1</v>
@@ -1351,16 +1351,16 @@
         <v>1</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E34">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34">
         <v>2</v>
       </c>
       <c r="G34">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -1380,16 +1380,16 @@
         <v>1</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E35">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35">
         <v>3</v>
       </c>
       <c r="G35">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H35">
         <v>1</v>
@@ -1409,16 +1409,16 @@
         <v>1</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E36">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F36">
         <v>4</v>
       </c>
       <c r="G36">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H36">
         <v>1</v>
@@ -1438,16 +1438,16 @@
         <v>1</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E37">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37">
         <v>5</v>
       </c>
       <c r="G37">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H37">
         <v>1</v>
@@ -1467,7 +1467,7 @@
         <v>1</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E38">
         <v>4</v>
@@ -1476,7 +1476,7 @@
         <v>2</v>
       </c>
       <c r="G38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H38">
         <v>1</v>
@@ -1496,7 +1496,7 @@
         <v>1</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E39">
         <v>4</v>
@@ -1505,7 +1505,7 @@
         <v>3</v>
       </c>
       <c r="G39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H39">
         <v>1</v>
@@ -1525,7 +1525,7 @@
         <v>1</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E40">
         <v>4</v>
@@ -1534,7 +1534,7 @@
         <v>4</v>
       </c>
       <c r="G40">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H40">
         <v>1</v>
@@ -1554,7 +1554,7 @@
         <v>1</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E41">
         <v>4</v>
@@ -1563,7 +1563,7 @@
         <v>5</v>
       </c>
       <c r="G41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H41">
         <v>1</v>
@@ -1583,7 +1583,7 @@
         <v>1</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E42">
         <v>4</v>
@@ -1592,7 +1592,7 @@
         <v>2</v>
       </c>
       <c r="G42">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H42">
         <v>1</v>
@@ -1612,7 +1612,7 @@
         <v>1</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E43">
         <v>4</v>
@@ -1621,7 +1621,7 @@
         <v>3</v>
       </c>
       <c r="G43">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H43">
         <v>1</v>
@@ -1641,7 +1641,7 @@
         <v>1</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E44">
         <v>4</v>
@@ -1650,7 +1650,7 @@
         <v>4</v>
       </c>
       <c r="G44">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -1670,7 +1670,7 @@
         <v>1</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E45">
         <v>4</v>
@@ -1679,7 +1679,7 @@
         <v>5</v>
       </c>
       <c r="G45">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H45">
         <v>1</v>
@@ -1699,7 +1699,7 @@
         <v>1</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E46">
         <v>4</v>
@@ -1708,7 +1708,7 @@
         <v>2</v>
       </c>
       <c r="G46">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H46">
         <v>1</v>
@@ -1728,7 +1728,7 @@
         <v>1</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E47">
         <v>4</v>
@@ -1737,7 +1737,7 @@
         <v>3</v>
       </c>
       <c r="G47">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H47">
         <v>1</v>
@@ -1757,7 +1757,7 @@
         <v>1</v>
       </c>
       <c r="D48">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E48">
         <v>4</v>
@@ -1766,7 +1766,7 @@
         <v>4</v>
       </c>
       <c r="G48">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H48">
         <v>1</v>
@@ -1786,7 +1786,7 @@
         <v>1</v>
       </c>
       <c r="D49">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E49">
         <v>4</v>
@@ -1795,7 +1795,7 @@
         <v>5</v>
       </c>
       <c r="G49">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H49">
         <v>1</v>
@@ -1804,8 +1804,1052 @@
         <v>1</v>
       </c>
     </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>4</v>
+      </c>
+      <c r="E50">
+        <v>4</v>
+      </c>
+      <c r="F50">
+        <v>2</v>
+      </c>
+      <c r="G50">
+        <v>5</v>
+      </c>
+      <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>4</v>
+      </c>
+      <c r="E51">
+        <v>4</v>
+      </c>
+      <c r="F51">
+        <v>3</v>
+      </c>
+      <c r="G51">
+        <v>5</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>4</v>
+      </c>
+      <c r="E52">
+        <v>4</v>
+      </c>
+      <c r="F52">
+        <v>4</v>
+      </c>
+      <c r="G52">
+        <v>5</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>4</v>
+      </c>
+      <c r="E53">
+        <v>4</v>
+      </c>
+      <c r="F53">
+        <v>5</v>
+      </c>
+      <c r="G53">
+        <v>5</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>3</v>
+      </c>
+      <c r="F54">
+        <v>2</v>
+      </c>
+      <c r="G54">
+        <v>2</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>3</v>
+      </c>
+      <c r="F55">
+        <v>3</v>
+      </c>
+      <c r="G55">
+        <v>2</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="I55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>1</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>3</v>
+      </c>
+      <c r="F56">
+        <v>4</v>
+      </c>
+      <c r="G56">
+        <v>2</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="I56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>3</v>
+      </c>
+      <c r="F57">
+        <v>5</v>
+      </c>
+      <c r="G57">
+        <v>2</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+      <c r="F58">
+        <v>2</v>
+      </c>
+      <c r="G58">
+        <v>3</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="I58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>3</v>
+      </c>
+      <c r="F59">
+        <v>3</v>
+      </c>
+      <c r="G59">
+        <v>3</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>3</v>
+      </c>
+      <c r="F60">
+        <v>4</v>
+      </c>
+      <c r="G60">
+        <v>3</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>3</v>
+      </c>
+      <c r="F61">
+        <v>5</v>
+      </c>
+      <c r="G61">
+        <v>3</v>
+      </c>
+      <c r="H61">
+        <v>1</v>
+      </c>
+      <c r="I61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>3</v>
+      </c>
+      <c r="F62">
+        <v>2</v>
+      </c>
+      <c r="G62">
+        <v>4</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="I62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>3</v>
+      </c>
+      <c r="F63">
+        <v>3</v>
+      </c>
+      <c r="G63">
+        <v>4</v>
+      </c>
+      <c r="H63">
+        <v>1</v>
+      </c>
+      <c r="I63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>3</v>
+      </c>
+      <c r="F64">
+        <v>4</v>
+      </c>
+      <c r="G64">
+        <v>4</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>1</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>3</v>
+      </c>
+      <c r="F65">
+        <v>5</v>
+      </c>
+      <c r="G65">
+        <v>4</v>
+      </c>
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="I65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>1</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>3</v>
+      </c>
+      <c r="F66">
+        <v>2</v>
+      </c>
+      <c r="G66">
+        <v>5</v>
+      </c>
+      <c r="H66">
+        <v>1</v>
+      </c>
+      <c r="I66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>1</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>3</v>
+      </c>
+      <c r="F67">
+        <v>3</v>
+      </c>
+      <c r="G67">
+        <v>5</v>
+      </c>
+      <c r="H67">
+        <v>1</v>
+      </c>
+      <c r="I67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>1</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>3</v>
+      </c>
+      <c r="F68">
+        <v>4</v>
+      </c>
+      <c r="G68">
+        <v>5</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+      <c r="I68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>1</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <v>3</v>
+      </c>
+      <c r="F69">
+        <v>5</v>
+      </c>
+      <c r="G69">
+        <v>5</v>
+      </c>
+      <c r="H69">
+        <v>1</v>
+      </c>
+      <c r="I69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>1</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>4</v>
+      </c>
+      <c r="F70">
+        <v>2</v>
+      </c>
+      <c r="G70">
+        <v>2</v>
+      </c>
+      <c r="H70">
+        <v>1</v>
+      </c>
+      <c r="I70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>1</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>4</v>
+      </c>
+      <c r="F71">
+        <v>3</v>
+      </c>
+      <c r="G71">
+        <v>2</v>
+      </c>
+      <c r="H71">
+        <v>1</v>
+      </c>
+      <c r="I71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>1</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>4</v>
+      </c>
+      <c r="F72">
+        <v>4</v>
+      </c>
+      <c r="G72">
+        <v>2</v>
+      </c>
+      <c r="H72">
+        <v>1</v>
+      </c>
+      <c r="I72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>1</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>4</v>
+      </c>
+      <c r="F73">
+        <v>5</v>
+      </c>
+      <c r="G73">
+        <v>2</v>
+      </c>
+      <c r="H73">
+        <v>1</v>
+      </c>
+      <c r="I73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>1</v>
+      </c>
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74">
+        <v>4</v>
+      </c>
+      <c r="F74">
+        <v>2</v>
+      </c>
+      <c r="G74">
+        <v>3</v>
+      </c>
+      <c r="H74">
+        <v>1</v>
+      </c>
+      <c r="I74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>1</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <v>4</v>
+      </c>
+      <c r="F75">
+        <v>3</v>
+      </c>
+      <c r="G75">
+        <v>3</v>
+      </c>
+      <c r="H75">
+        <v>1</v>
+      </c>
+      <c r="I75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>1</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76">
+        <v>4</v>
+      </c>
+      <c r="F76">
+        <v>4</v>
+      </c>
+      <c r="G76">
+        <v>3</v>
+      </c>
+      <c r="H76">
+        <v>1</v>
+      </c>
+      <c r="I76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>1</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <v>4</v>
+      </c>
+      <c r="F77">
+        <v>5</v>
+      </c>
+      <c r="G77">
+        <v>3</v>
+      </c>
+      <c r="H77">
+        <v>1</v>
+      </c>
+      <c r="I77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>1</v>
+      </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="E78">
+        <v>4</v>
+      </c>
+      <c r="F78">
+        <v>2</v>
+      </c>
+      <c r="G78">
+        <v>4</v>
+      </c>
+      <c r="H78">
+        <v>1</v>
+      </c>
+      <c r="I78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>1</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <v>4</v>
+      </c>
+      <c r="F79">
+        <v>3</v>
+      </c>
+      <c r="G79">
+        <v>4</v>
+      </c>
+      <c r="H79">
+        <v>1</v>
+      </c>
+      <c r="I79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>1</v>
+      </c>
+      <c r="B80">
+        <v>1</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+      <c r="E80">
+        <v>4</v>
+      </c>
+      <c r="F80">
+        <v>4</v>
+      </c>
+      <c r="G80">
+        <v>4</v>
+      </c>
+      <c r="H80">
+        <v>1</v>
+      </c>
+      <c r="I80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>1</v>
+      </c>
+      <c r="B81">
+        <v>1</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+      <c r="E81">
+        <v>4</v>
+      </c>
+      <c r="F81">
+        <v>5</v>
+      </c>
+      <c r="G81">
+        <v>4</v>
+      </c>
+      <c r="H81">
+        <v>1</v>
+      </c>
+      <c r="I81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>1</v>
+      </c>
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="C82">
+        <v>1</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+      <c r="E82">
+        <v>4</v>
+      </c>
+      <c r="F82">
+        <v>2</v>
+      </c>
+      <c r="G82">
+        <v>5</v>
+      </c>
+      <c r="H82">
+        <v>1</v>
+      </c>
+      <c r="I82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>1</v>
+      </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
+      <c r="C83">
+        <v>1</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83">
+        <v>4</v>
+      </c>
+      <c r="F83">
+        <v>3</v>
+      </c>
+      <c r="G83">
+        <v>5</v>
+      </c>
+      <c r="H83">
+        <v>1</v>
+      </c>
+      <c r="I83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>1</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+      <c r="C84">
+        <v>1</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+      <c r="E84">
+        <v>4</v>
+      </c>
+      <c r="F84">
+        <v>4</v>
+      </c>
+      <c r="G84">
+        <v>5</v>
+      </c>
+      <c r="H84">
+        <v>1</v>
+      </c>
+      <c r="I84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>1</v>
+      </c>
+      <c r="B85">
+        <v>1</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85">
+        <v>4</v>
+      </c>
+      <c r="F85">
+        <v>5</v>
+      </c>
+      <c r="G85">
+        <v>5</v>
+      </c>
+      <c r="H85">
+        <v>1</v>
+      </c>
+      <c r="I85">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="E1:E49"/>
+  <autoFilter ref="E1:E53"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>